<commit_message>
updated model names in excel file
</commit_message>
<xml_diff>
--- a/multimodel_inference/moments_multimodels.xlsx
+++ b/multimodel_inference/moments_multimodels.xlsx
@@ -29,24 +29,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="141">
   <si>
-    <t>SC3ie</t>
-  </si>
-  <si>
-    <t>SC3im</t>
-  </si>
-  <si>
-    <t>SC3il</t>
-  </si>
-  <si>
-    <t>SC3iml</t>
-  </si>
-  <si>
-    <t>SC3iem</t>
-  </si>
-  <si>
-    <t>SC3iel</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -74,222 +56,24 @@
     <t>symmetric migration?</t>
   </si>
   <si>
-    <t>SC3iesm</t>
-  </si>
-  <si>
-    <t>SC3imsm</t>
-  </si>
-  <si>
-    <t>SC3ilsm</t>
-  </si>
-  <si>
-    <t>SC3imlsm</t>
-  </si>
-  <si>
-    <t>SC3iemsm</t>
-  </si>
-  <si>
-    <t>SC3ielsm</t>
-  </si>
-  <si>
-    <t>SC3e</t>
-  </si>
-  <si>
-    <t>SC3m</t>
-  </si>
-  <si>
-    <t>SC3l</t>
-  </si>
-  <si>
-    <t>SC3ml</t>
-  </si>
-  <si>
-    <t>SC3em</t>
-  </si>
-  <si>
-    <t>SC3el</t>
-  </si>
-  <si>
-    <t>SC3esm</t>
-  </si>
-  <si>
-    <t>SC3msm</t>
-  </si>
-  <si>
-    <t>SC3lsm</t>
-  </si>
-  <si>
-    <t>SC3mlsm</t>
-  </si>
-  <si>
-    <t>SC3emsm</t>
-  </si>
-  <si>
-    <t>SC3elsm</t>
-  </si>
-  <si>
-    <t>SC2ie</t>
-  </si>
-  <si>
-    <t>SC2il</t>
-  </si>
-  <si>
-    <t>SC2e</t>
-  </si>
-  <si>
-    <t>SC2iesm</t>
-  </si>
-  <si>
-    <t>SC2ilsm</t>
-  </si>
-  <si>
-    <t>SC1i</t>
-  </si>
-  <si>
-    <t>SC1</t>
-  </si>
-  <si>
-    <t>SC2l</t>
-  </si>
-  <si>
-    <t>SC2esm</t>
-  </si>
-  <si>
-    <t>SC2lsm</t>
-  </si>
-  <si>
-    <t>SC1nm</t>
-  </si>
-  <si>
-    <t>SC2nm</t>
-  </si>
-  <si>
-    <t>SC3nm</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>SC1ns</t>
-  </si>
-  <si>
-    <t>SC2ns</t>
-  </si>
-  <si>
-    <t>SC3ns</t>
-  </si>
-  <si>
-    <t>Imi</t>
-  </si>
-  <si>
-    <t>Imsm</t>
-  </si>
-  <si>
-    <t>Imism</t>
-  </si>
-  <si>
-    <t>Imsc</t>
-  </si>
-  <si>
-    <t>Imscsm</t>
-  </si>
-  <si>
-    <t>Im</t>
-  </si>
-  <si>
-    <t>Imnm</t>
-  </si>
-  <si>
-    <t>Imscnm</t>
-  </si>
-  <si>
-    <t>Imns</t>
-  </si>
-  <si>
-    <t>Imscns</t>
-  </si>
-  <si>
-    <t>SC1ie</t>
-  </si>
-  <si>
-    <t>SC1il</t>
-  </si>
-  <si>
     <t>1 early</t>
   </si>
   <si>
     <t>1 late</t>
   </si>
   <si>
-    <t>SC1iesm</t>
-  </si>
-  <si>
-    <t>SC1ilsm</t>
-  </si>
-  <si>
-    <t>SC1e</t>
-  </si>
-  <si>
-    <t>SC1l</t>
-  </si>
-  <si>
-    <t>SC1esm</t>
-  </si>
-  <si>
-    <t>SC1lsm</t>
-  </si>
-  <si>
     <t>1,2,3</t>
   </si>
   <si>
-    <t>SC3ieml</t>
-  </si>
-  <si>
-    <t>SC3iemlsm</t>
-  </si>
-  <si>
-    <t>SC3eml</t>
-  </si>
-  <si>
-    <t>SC3emlsm</t>
-  </si>
-  <si>
-    <t>SC2iel</t>
-  </si>
-  <si>
-    <t>SC2ielsm</t>
-  </si>
-  <si>
-    <t>SC2el</t>
-  </si>
-  <si>
-    <t>SC2elsm</t>
-  </si>
-  <si>
-    <t>SC3ielsm1</t>
-  </si>
-  <si>
-    <t>SC3ielsm2</t>
-  </si>
-  <si>
-    <t>SC3imlsm2</t>
-  </si>
-  <si>
     <t>no in 2nd epoch, yes in 3d epoch</t>
   </si>
   <si>
     <t>yes in 2nd epoch, no in 3d epoch</t>
   </si>
   <si>
-    <t>SC3imlsm1</t>
-  </si>
-  <si>
-    <t>SC3iemsm1</t>
-  </si>
-  <si>
-    <t>SC3iemsm2</t>
-  </si>
-  <si>
     <t>no in 1st epoch, yes in 2nd epoch</t>
   </si>
   <si>
@@ -302,102 +86,30 @@
     <t>no in 1st epoch, yes in 3d epoch</t>
   </si>
   <si>
-    <t>SC12im</t>
-  </si>
-  <si>
-    <t>SC12il</t>
-  </si>
-  <si>
-    <t>SC12iml</t>
-  </si>
-  <si>
     <t>1before split, then 2</t>
   </si>
   <si>
-    <t>SC12imlsm</t>
-  </si>
-  <si>
-    <t>SC12imsm</t>
-  </si>
-  <si>
-    <t>SC12ilsm</t>
-  </si>
-  <si>
-    <t>SC12ilmsm1</t>
-  </si>
-  <si>
-    <t>SC12ilmsm2</t>
-  </si>
-  <si>
-    <t>SC11nm</t>
-  </si>
-  <si>
     <t>1before split, 1 after</t>
   </si>
   <si>
-    <t>SC12nm</t>
-  </si>
-  <si>
     <t>1before split, 2 after</t>
   </si>
   <si>
-    <t>SC21nm</t>
-  </si>
-  <si>
     <t>2before split, 1 after</t>
   </si>
   <si>
-    <t>SC2ielsm1</t>
-  </si>
-  <si>
-    <t>SC2ielsm2</t>
-  </si>
-  <si>
-    <t>SC1ielsm1</t>
-  </si>
-  <si>
-    <t>SC1ielsm2</t>
-  </si>
-  <si>
     <t>1 early and late, independent</t>
   </si>
   <si>
-    <t>SC2i</t>
-  </si>
-  <si>
     <t>1,2 same</t>
   </si>
   <si>
     <t>1,2 different</t>
   </si>
   <si>
-    <t>Imisc</t>
-  </si>
-  <si>
-    <t>Imiscsm</t>
-  </si>
-  <si>
-    <t>Imisc2</t>
-  </si>
-  <si>
     <t>2, free size of 1st epoch</t>
   </si>
   <si>
-    <t>Imisc2sm</t>
-  </si>
-  <si>
-    <t>Imsc2</t>
-  </si>
-  <si>
-    <t>SC3ml2</t>
-  </si>
-  <si>
-    <t>SC3em2</t>
-  </si>
-  <si>
-    <t>SC3el2</t>
-  </si>
-  <si>
     <t>1,3 independent</t>
   </si>
   <si>
@@ -407,33 +119,12 @@
     <t>1,2 independent</t>
   </si>
   <si>
-    <t>SC2</t>
-  </si>
-  <si>
-    <t>SC2sm1</t>
-  </si>
-  <si>
-    <t>SC2sm2</t>
-  </si>
-  <si>
-    <t>SC11</t>
-  </si>
-  <si>
-    <t>SC11sm</t>
-  </si>
-  <si>
-    <t>SC1sm1</t>
-  </si>
-  <si>
     <t>yes early, no late</t>
   </si>
   <si>
     <t>no early, yes late</t>
   </si>
   <si>
-    <t>SC1sm2</t>
-  </si>
-  <si>
     <t>s2m</t>
   </si>
   <si>
@@ -449,7 +140,316 @@
     <t>1 for  background genome, 0 for  islands</t>
   </si>
   <si>
-    <t>ImscsmB</t>
+    <t>IM</t>
+  </si>
+  <si>
+    <t>IMi</t>
+  </si>
+  <si>
+    <t>IMsm</t>
+  </si>
+  <si>
+    <t>IMism</t>
+  </si>
+  <si>
+    <t>IMsc</t>
+  </si>
+  <si>
+    <t>IMsc2</t>
+  </si>
+  <si>
+    <t>IMisc</t>
+  </si>
+  <si>
+    <t>IMisc2</t>
+  </si>
+  <si>
+    <t>IMscsm</t>
+  </si>
+  <si>
+    <t>IMscsmB</t>
+  </si>
+  <si>
+    <t>IMiscsm</t>
+  </si>
+  <si>
+    <t>IMisc2sm</t>
+  </si>
+  <si>
+    <t>IMnm</t>
+  </si>
+  <si>
+    <t>IMscnm</t>
+  </si>
+  <si>
+    <t>IMns</t>
+  </si>
+  <si>
+    <t>IMscns</t>
+  </si>
+  <si>
+    <t>sc3ie</t>
+  </si>
+  <si>
+    <t>sc3im</t>
+  </si>
+  <si>
+    <t>sc3il</t>
+  </si>
+  <si>
+    <t>sc12iml</t>
+  </si>
+  <si>
+    <t>sc12im</t>
+  </si>
+  <si>
+    <t>sc12il</t>
+  </si>
+  <si>
+    <t>sc12imlsm</t>
+  </si>
+  <si>
+    <t>sc12imsm</t>
+  </si>
+  <si>
+    <t>sc12ilsm</t>
+  </si>
+  <si>
+    <t>sc12ilmsm1</t>
+  </si>
+  <si>
+    <t>sc12ilmsm2</t>
+  </si>
+  <si>
+    <t>sc3ieml</t>
+  </si>
+  <si>
+    <t>sc3iml</t>
+  </si>
+  <si>
+    <t>sc3iem</t>
+  </si>
+  <si>
+    <t>sc3iel</t>
+  </si>
+  <si>
+    <t>sc3ielsm1</t>
+  </si>
+  <si>
+    <t>sc3ielsm2</t>
+  </si>
+  <si>
+    <t>sc3iemsm1</t>
+  </si>
+  <si>
+    <t>sc3iemsm2</t>
+  </si>
+  <si>
+    <t>sc3imlsm2</t>
+  </si>
+  <si>
+    <t>sc3imlsm1</t>
+  </si>
+  <si>
+    <t>sc3iesm</t>
+  </si>
+  <si>
+    <t>sc3imsm</t>
+  </si>
+  <si>
+    <t>sc3ilsm</t>
+  </si>
+  <si>
+    <t>sc3iemlsm</t>
+  </si>
+  <si>
+    <t>sc3imlsm</t>
+  </si>
+  <si>
+    <t>sc3iemsm</t>
+  </si>
+  <si>
+    <t>sc3ielsm</t>
+  </si>
+  <si>
+    <t>sc3e</t>
+  </si>
+  <si>
+    <t>sc3m</t>
+  </si>
+  <si>
+    <t>sc3l</t>
+  </si>
+  <si>
+    <t>sc3eml</t>
+  </si>
+  <si>
+    <t>sc3ml</t>
+  </si>
+  <si>
+    <t>sc3em</t>
+  </si>
+  <si>
+    <t>sc3el</t>
+  </si>
+  <si>
+    <t>sc3ml2</t>
+  </si>
+  <si>
+    <t>sc3em2</t>
+  </si>
+  <si>
+    <t>sc3el2</t>
+  </si>
+  <si>
+    <t>sc3esm</t>
+  </si>
+  <si>
+    <t>sc3msm</t>
+  </si>
+  <si>
+    <t>sc3lsm</t>
+  </si>
+  <si>
+    <t>sc3emlsm</t>
+  </si>
+  <si>
+    <t>sc3mlsm</t>
+  </si>
+  <si>
+    <t>sc3emsm</t>
+  </si>
+  <si>
+    <t>sc3elsm</t>
+  </si>
+  <si>
+    <t>sc2i</t>
+  </si>
+  <si>
+    <t>sc2ie</t>
+  </si>
+  <si>
+    <t>sc2il</t>
+  </si>
+  <si>
+    <t>sc2iel</t>
+  </si>
+  <si>
+    <t>sc2iesm</t>
+  </si>
+  <si>
+    <t>sc2ilsm</t>
+  </si>
+  <si>
+    <t>sc2ielsm</t>
+  </si>
+  <si>
+    <t>sc2ielsm1</t>
+  </si>
+  <si>
+    <t>sc2ielsm2</t>
+  </si>
+  <si>
+    <t>sc2</t>
+  </si>
+  <si>
+    <t>sc2sm1</t>
+  </si>
+  <si>
+    <t>sc2sm2</t>
+  </si>
+  <si>
+    <t>sc2e</t>
+  </si>
+  <si>
+    <t>sc2l</t>
+  </si>
+  <si>
+    <t>sc2el</t>
+  </si>
+  <si>
+    <t>sc2esm</t>
+  </si>
+  <si>
+    <t>sc2lsm</t>
+  </si>
+  <si>
+    <t>sc2elsm</t>
+  </si>
+  <si>
+    <t>sc11</t>
+  </si>
+  <si>
+    <t>sc11sm</t>
+  </si>
+  <si>
+    <t>sc1ie</t>
+  </si>
+  <si>
+    <t>sc1il</t>
+  </si>
+  <si>
+    <t>sc1iesm</t>
+  </si>
+  <si>
+    <t>sc1ielsm1</t>
+  </si>
+  <si>
+    <t>sc1ielsm2</t>
+  </si>
+  <si>
+    <t>sc1ilsm</t>
+  </si>
+  <si>
+    <t>sc1e</t>
+  </si>
+  <si>
+    <t>sc1l</t>
+  </si>
+  <si>
+    <t>sc1esm</t>
+  </si>
+  <si>
+    <t>sc1lsm</t>
+  </si>
+  <si>
+    <t>sc1i</t>
+  </si>
+  <si>
+    <t>sc1</t>
+  </si>
+  <si>
+    <t>sc1sm1</t>
+  </si>
+  <si>
+    <t>sc1sm2</t>
+  </si>
+  <si>
+    <t>sc11nm</t>
+  </si>
+  <si>
+    <t>sc12nm</t>
+  </si>
+  <si>
+    <t>sc21nm</t>
+  </si>
+  <si>
+    <t>sc1nm</t>
+  </si>
+  <si>
+    <t>sc2nm</t>
+  </si>
+  <si>
+    <t>sc3nm</t>
+  </si>
+  <si>
+    <t>sc1ns</t>
+  </si>
+  <si>
+    <t>sc2ns</t>
+  </si>
+  <si>
+    <t>sc3ns</t>
   </si>
 </sst>
 </file>
@@ -766,35 +766,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -814,7 +817,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -834,7 +837,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -854,19 +857,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -874,13 +877,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -894,13 +897,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -914,19 +917,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -934,13 +937,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -954,13 +957,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -974,13 +977,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -989,18 +992,18 @@
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1009,12 +1012,12 @@
         <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1026,7 +1029,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1034,7 +1037,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1046,7 +1049,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1054,7 +1057,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1066,7 +1069,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1074,7 +1077,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1086,7 +1089,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1094,7 +1097,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1106,15 +1109,15 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1126,15 +1129,15 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1146,15 +1149,15 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1166,15 +1169,15 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>87</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1186,15 +1189,15 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F21" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1206,15 +1209,15 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1234,7 +1237,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1254,7 +1257,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1274,7 +1277,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1286,7 +1289,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1294,7 +1297,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -1306,7 +1309,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1314,7 +1317,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1326,7 +1329,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1334,7 +1337,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1346,7 +1349,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1354,7 +1357,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -1374,7 +1377,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1394,7 +1397,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1414,7 +1417,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -1426,7 +1429,7 @@
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -1434,7 +1437,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1446,7 +1449,7 @@
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1454,7 +1457,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -1466,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1474,7 +1477,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -1486,7 +1489,7 @@
         <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -1494,7 +1497,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -1506,7 +1509,7 @@
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>124</v>
+        <v>28</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1514,7 +1517,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>121</v>
+        <v>89</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -1526,7 +1529,7 @@
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>125</v>
+        <v>29</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -1534,7 +1537,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -1546,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>123</v>
+        <v>27</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1554,7 +1557,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -1574,7 +1577,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -1594,7 +1597,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -1614,7 +1617,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -1626,7 +1629,7 @@
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -1634,7 +1637,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -1646,7 +1649,7 @@
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -1654,7 +1657,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -1666,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -1674,7 +1677,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -1686,7 +1689,7 @@
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -1694,7 +1697,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -1706,7 +1709,7 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -1714,7 +1717,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -1734,7 +1737,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -1754,7 +1757,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -1766,7 +1769,7 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -1774,7 +1777,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -1794,7 +1797,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -1814,7 +1817,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -1826,7 +1829,7 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -1834,7 +1837,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -1846,15 +1849,15 @@
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F54" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -1866,15 +1869,15 @@
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F55" t="s">
-        <v>87</v>
+        <v>15</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -1886,7 +1889,7 @@
         <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>125</v>
+        <v>29</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -1894,7 +1897,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -1906,15 +1909,15 @@
         <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>125</v>
+        <v>29</v>
       </c>
       <c r="F57" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -1926,15 +1929,15 @@
         <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>125</v>
+        <v>29</v>
       </c>
       <c r="F58" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -1954,7 +1957,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -1974,7 +1977,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -1986,7 +1989,7 @@
         <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -1994,7 +1997,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -2014,7 +2017,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -2034,7 +2037,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -2046,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="E64" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -2054,13 +2057,13 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -2074,13 +2077,13 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B66">
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -2094,7 +2097,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -2106,7 +2109,7 @@
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="F67">
         <v>0</v>
@@ -2114,7 +2117,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -2126,7 +2129,7 @@
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="F68">
         <v>0</v>
@@ -2134,7 +2137,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2146,7 +2149,7 @@
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -2154,7 +2157,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -2169,12 +2172,12 @@
         <v>1</v>
       </c>
       <c r="F70" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2189,12 +2192,12 @@
         <v>1</v>
       </c>
       <c r="F71" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2206,7 +2209,7 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -2214,7 +2217,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -2226,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="F73">
         <v>0</v>
@@ -2234,7 +2237,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2246,7 +2249,7 @@
         <v>0</v>
       </c>
       <c r="E74" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="F74">
         <v>0</v>
@@ -2254,7 +2257,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2266,7 +2269,7 @@
         <v>0</v>
       </c>
       <c r="E75" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="F75">
         <v>1</v>
@@ -2274,7 +2277,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>69</v>
+        <v>127</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2286,7 +2289,7 @@
         <v>0</v>
       </c>
       <c r="E76" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="F76">
         <v>1</v>
@@ -2294,7 +2297,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>38</v>
+        <v>128</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -2306,7 +2309,7 @@
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="F77">
         <v>0</v>
@@ -2314,7 +2317,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>39</v>
+        <v>129</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -2326,7 +2329,7 @@
         <v>0</v>
       </c>
       <c r="E78" t="s">
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="F78">
         <v>0</v>
@@ -2334,7 +2337,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -2346,15 +2349,15 @@
         <v>0</v>
       </c>
       <c r="E79" t="s">
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="F79" t="s">
-        <v>132</v>
+        <v>30</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -2366,75 +2369,75 @@
         <v>0</v>
       </c>
       <c r="E80" t="s">
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="F80" t="s">
-        <v>133</v>
+        <v>31</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="B81">
         <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
       <c r="D81" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="E81" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="F81" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="B82">
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>103</v>
+        <v>21</v>
       </c>
       <c r="D82" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="E82" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="F82" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="B83">
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="D83" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="E83" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="F83" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>43</v>
+        <v>135</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -2443,18 +2446,18 @@
         <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="E84" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="F84" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>44</v>
+        <v>136</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -2463,18 +2466,18 @@
         <v>2</v>
       </c>
       <c r="D85" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="E85" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="F85" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>45</v>
+        <v>137</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -2483,18 +2486,18 @@
         <v>3</v>
       </c>
       <c r="D86" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="E86" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="F86" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>47</v>
+        <v>138</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -2503,18 +2506,18 @@
         <v>1</v>
       </c>
       <c r="D87" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="E87" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="F87" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>48</v>
+        <v>139</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -2523,18 +2526,18 @@
         <v>2</v>
       </c>
       <c r="D88" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="E88" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="F88" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>49</v>
+        <v>140</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -2543,18 +2546,18 @@
         <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="E89" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="F89" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>135</v>
+        <v>32</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -2574,7 +2577,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>136</v>
+        <v>33</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -2594,7 +2597,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>137</v>
+        <v>34</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -2614,7 +2617,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>138</v>
+        <v>35</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -2629,12 +2632,12 @@
         <v>1</v>
       </c>
       <c r="F93" t="s">
-        <v>139</v>
+        <v>36</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -2654,7 +2657,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -2674,7 +2677,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -2694,7 +2697,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -2714,7 +2717,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -2734,13 +2737,13 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>119</v>
+        <v>42</v>
       </c>
       <c r="B99">
         <v>1</v>
       </c>
       <c r="C99" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -2754,7 +2757,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>114</v>
+        <v>43</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -2774,13 +2777,13 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>116</v>
+        <v>44</v>
       </c>
       <c r="B101">
         <v>1</v>
       </c>
       <c r="C101" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="D101">
         <v>1</v>
@@ -2794,7 +2797,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B102">
         <v>1</v>
@@ -2814,7 +2817,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>140</v>
+        <v>46</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -2829,12 +2832,12 @@
         <v>1</v>
       </c>
       <c r="F103" t="s">
-        <v>139</v>
+        <v>36</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>115</v>
+        <v>47</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -2854,13 +2857,13 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>118</v>
+        <v>48</v>
       </c>
       <c r="B105">
         <v>1</v>
       </c>
       <c r="C105" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="D105">
         <v>1</v>
@@ -2874,7 +2877,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B106">
         <v>1</v>
@@ -2886,15 +2889,15 @@
         <v>0</v>
       </c>
       <c r="E106" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="F106" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -2906,15 +2909,15 @@
         <v>0</v>
       </c>
       <c r="E107" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="F107" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -2923,18 +2926,18 @@
         <v>1</v>
       </c>
       <c r="D108" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="E108" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="F108" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -2943,13 +2946,13 @@
         <v>2</v>
       </c>
       <c r="D109" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="E109" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="F109" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>